<commit_message>
Add experiment 0 new outputs
</commit_message>
<xml_diff>
--- a/experiments/experiment_0/outputs/train_results.xlsx
+++ b/experiments/experiment_0/outputs/train_results.xlsx
@@ -490,22 +490,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5047528523613106</v>
+        <v>0.5036030259322036</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.002376259668327288</v>
+        <v>-0.003301823931420644</v>
       </c>
       <c r="D2" t="n">
-        <v>0.07948332140373796</v>
+        <v>0.09737528968779639</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5093426641808255</v>
+        <v>0.5088895124359837</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1954832419720788</v>
+        <v>0.2009876593974531</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4123034070838582</v>
+        <v>0.4114699837836353</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -514,10 +514,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5286362690215993</v>
+        <v>0.5396786495508421</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1762120896738665</v>
+        <v>0.179892883183614</v>
       </c>
     </row>
     <row r="3">
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3795108199119568</v>
+        <v>0.3790133937515996</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -534,13 +534,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5448047368696486</v>
+        <v>0.5457309037138974</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1816015789565495</v>
+        <v>0.1819103012379658</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3799817575649782</v>
+        <v>0.3785203017971732</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -549,10 +549,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5489083043196299</v>
+        <v>0.5578166024369045</v>
       </c>
       <c r="K3" t="n">
-        <v>0.18296943477321</v>
+        <v>0.1859388674789682</v>
       </c>
     </row>
     <row r="4">
@@ -560,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3608096617866646</v>
+        <v>0.3604567447169261</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -569,13 +569,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5658470243145279</v>
+        <v>0.5666659506688142</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1886156747715093</v>
+        <v>0.1888886502229381</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3696851066567681</v>
+        <v>0.3686447604136033</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -584,10 +584,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5637311178658796</v>
+        <v>0.5714342616015085</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1879103726219599</v>
+        <v>0.1904780872005028</v>
       </c>
     </row>
     <row r="5">
@@ -595,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3533276888457211</v>
+        <v>0.3530302684415471</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -604,13 +604,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5847626012949111</v>
+        <v>0.5853264494650416</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1949208670983037</v>
+        <v>0.1951088164883472</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3618033514781432</v>
+        <v>0.3606859147548676</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -619,10 +619,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5722867110888844</v>
+        <v>0.5796229680564096</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1907622370296281</v>
+        <v>0.1932076560188032</v>
       </c>
     </row>
     <row r="6">
@@ -630,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3501529219475659</v>
+        <v>0.3499245823106982</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -639,13 +639,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5981007920470348</v>
+        <v>0.5954577301728151</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1993669306823449</v>
+        <v>0.198485910057605</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3578439734198831</v>
+        <v>0.3569470725276254</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -654,10 +654,10 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5786047453803909</v>
+        <v>0.5863773971814888</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1928682484601303</v>
+        <v>0.1954591323938296</v>
       </c>
     </row>
     <row r="7">
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3472056788477031</v>
+        <v>0.3470941765064543</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -674,13 +674,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6101892503869507</v>
+        <v>0.6068835801303305</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2033964167956502</v>
+        <v>0.2022945267101102</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3554728383367712</v>
+        <v>0.354636090722951</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -689,10 +689,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5846349599274261</v>
+        <v>0.5903205122162741</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1948783199758087</v>
+        <v>0.1967735040720914</v>
       </c>
     </row>
     <row r="8">
@@ -700,34 +700,34 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3452996794473041</v>
+        <v>0.3449262163855813</v>
       </c>
       <c r="C8" t="n">
-        <v>-8.950643255542512e-05</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6157029337625677</v>
+        <v>0.6155885236437774</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2052044757766708</v>
+        <v>0.2051961745479258</v>
       </c>
       <c r="G8" t="n">
-        <v>0.355294482274489</v>
+        <v>0.3543762605298649</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0003886501516683488</v>
+        <v>0.0007468638049546311</v>
       </c>
       <c r="I8" t="n">
-        <v>0.002405893374212229</v>
+        <v>0.002416492023437834</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5925598304180089</v>
+        <v>0.5958452664436593</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1984514579812965</v>
+        <v>0.1996695407573506</v>
       </c>
     </row>
     <row r="9">
@@ -735,34 +735,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3431906314058737</v>
+        <v>0.3430333377962763</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0002853632263376538</v>
+        <v>0.0006597965067594441</v>
       </c>
       <c r="D9" t="n">
-        <v>0.001215099156199852</v>
+        <v>0.002427515974306546</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6274145782493868</v>
+        <v>0.6242408694379459</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2096383468773081</v>
+        <v>0.209109393973004</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3525195785544135</v>
+        <v>0.3517367853359742</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0007468638049546311</v>
+        <v>0.001614280377821645</v>
       </c>
       <c r="I9" t="n">
-        <v>0.002416492023437834</v>
+        <v>0.004809421071556993</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5958349047556243</v>
+        <v>0.5983577625582349</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1996660868613389</v>
+        <v>0.2015938213358712</v>
       </c>
     </row>
     <row r="10">
@@ -770,34 +770,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3407610116357153</v>
+        <v>0.3404405777427283</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0009362650218521368</v>
+        <v>0.0005779872203968001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003031049438701393</v>
+        <v>0.003024380463038685</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6338425259746903</v>
+        <v>0.6342679178190669</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2126032801450813</v>
+        <v>0.2126234285008341</v>
       </c>
       <c r="G10" t="n">
-        <v>0.351874210617759</v>
+        <v>0.3508104587143118</v>
       </c>
       <c r="H10" t="n">
-        <v>0.002275278269226591</v>
+        <v>0.002387735912156005</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0117210190025724</v>
+        <v>0.009578032420029857</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5962575785777109</v>
+        <v>0.6023933490831226</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2034179586165033</v>
+        <v>0.2047863724717695</v>
       </c>
     </row>
     <row r="11">
@@ -805,34 +805,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3403633033687418</v>
+        <v>0.3402540643106807</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0004805474173117941</v>
+        <v>0.001878056524443311</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00242216902282129</v>
+        <v>0.00781537643467577</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6401859128875362</v>
+        <v>0.6384324117965973</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2143628764425564</v>
+        <v>0.2160419482519055</v>
       </c>
       <c r="G11" t="n">
-        <v>0.349056136879054</v>
+        <v>0.3482667261903936</v>
       </c>
       <c r="H11" t="n">
-        <v>0.001539388561829211</v>
+        <v>0.001896908509437509</v>
       </c>
       <c r="I11" t="n">
         <v>0.009417059044126838</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6034311730811637</v>
+        <v>0.6047014163494222</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2047958735623732</v>
+        <v>0.2053384613009955</v>
       </c>
     </row>
     <row r="12">
@@ -840,34 +840,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.3387310233983127</v>
+        <v>0.3387496725402095</v>
       </c>
       <c r="C12" t="n">
-        <v>0.002354076443401645</v>
+        <v>0.002999450341867008</v>
       </c>
       <c r="D12" t="n">
-        <v>0.009520906808319182</v>
+        <v>0.01186559885186832</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6450977728770942</v>
+        <v>0.6421779150922657</v>
       </c>
       <c r="F12" t="n">
-        <v>0.218990918709605</v>
+        <v>0.219014321428667</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3498540412295948</v>
+        <v>0.3489238348874179</v>
       </c>
       <c r="H12" t="n">
-        <v>0.004478499485870743</v>
+        <v>0.00357798736181511</v>
       </c>
       <c r="I12" t="n">
-        <v>0.02048503404101036</v>
+        <v>0.02067638729156823</v>
       </c>
       <c r="J12" t="n">
-        <v>0.6020540737796689</v>
+        <v>0.6045810749788292</v>
       </c>
       <c r="K12" t="n">
-        <v>0.2090058691021833</v>
+        <v>0.2096118165440708</v>
       </c>
     </row>
     <row r="13">
@@ -875,34 +875,34 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3378683636811646</v>
+        <v>0.3379128659990701</v>
       </c>
       <c r="C13" t="n">
-        <v>0.002334600836357878</v>
+        <v>0.002983108246293859</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00960731896052891</v>
+        <v>0.01371554824814717</v>
       </c>
       <c r="E13" t="n">
-        <v>0.649143735465654</v>
+        <v>0.6464815594924289</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2203618850875136</v>
+        <v>0.2210600719956233</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3535749817436392</v>
+        <v>0.3529845042662187</v>
       </c>
       <c r="H13" t="n">
-        <v>0.003115543372967239</v>
+        <v>0.00525022475277194</v>
       </c>
       <c r="I13" t="n">
-        <v>0.02785573422330097</v>
+        <v>0.03545719664808595</v>
       </c>
       <c r="J13" t="n">
-        <v>0.6099612024015671</v>
+        <v>0.6121870070118389</v>
       </c>
       <c r="K13" t="n">
-        <v>0.2136441599992784</v>
+        <v>0.2176314761375656</v>
       </c>
     </row>
     <row r="14">
@@ -910,34 +910,34 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.3358239477330988</v>
+        <v>0.3357561576095494</v>
       </c>
       <c r="C14" t="n">
-        <v>0.005199250394136962</v>
+        <v>0.005646266610267819</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01938808546060591</v>
+        <v>0.02180552583972491</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6563135044905147</v>
+        <v>0.6536037779427742</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2269669467817526</v>
+        <v>0.2270185234642557</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3446310650218617</v>
+        <v>0.3439517969434912</v>
       </c>
       <c r="H14" t="n">
-        <v>0.004504602618270542</v>
+        <v>0.003662198246052087</v>
       </c>
       <c r="I14" t="n">
-        <v>0.02643584044917534</v>
+        <v>0.02298227410669829</v>
       </c>
       <c r="J14" t="n">
-        <v>0.6087505233340751</v>
+        <v>0.6108790478343</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2132303221338403</v>
+        <v>0.2125078400623501</v>
       </c>
     </row>
     <row r="15">
@@ -945,34 +945,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3349062167108059</v>
+        <v>0.3351019112901254</v>
       </c>
       <c r="C15" t="n">
-        <v>0.004365043847377043</v>
+        <v>0.004806994851293309</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01778785205311539</v>
+        <v>0.02126712016957187</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6589250876680616</v>
+        <v>0.6555668716285511</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2270259945228513</v>
+        <v>0.2272136622164721</v>
       </c>
       <c r="G15" t="n">
-        <v>0.347194106741385</v>
+        <v>0.3460760848088698</v>
       </c>
       <c r="H15" t="n">
-        <v>0.002734778411399283</v>
+        <v>0.003240712216380837</v>
       </c>
       <c r="I15" t="n">
-        <v>0.02633009708737864</v>
+        <v>0.02269888851249864</v>
       </c>
       <c r="J15" t="n">
-        <v>0.6115770700378329</v>
+        <v>0.6146157472453796</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2135473151788703</v>
+        <v>0.213518449324753</v>
       </c>
     </row>
     <row r="16">
@@ -980,34 +980,34 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.3332460983233018</v>
+        <v>0.3331597145985473</v>
       </c>
       <c r="C16" t="n">
-        <v>0.004937372001749249</v>
+        <v>0.007547131505694971</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02096685800820338</v>
+        <v>0.02867924668747523</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6661545257817313</v>
+        <v>0.6638042815619669</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2306862519305613</v>
+        <v>0.2333435532517124</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3456682237711819</v>
+        <v>0.3447341241619803</v>
       </c>
       <c r="H16" t="n">
-        <v>0.004227655946626746</v>
+        <v>0.003486013271655819</v>
       </c>
       <c r="I16" t="n">
-        <v>0.02494558367088697</v>
+        <v>0.02304569614227253</v>
       </c>
       <c r="J16" t="n">
-        <v>0.6124591578478722</v>
+        <v>0.6159164583798072</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2138774658217953</v>
+        <v>0.2141493892645785</v>
       </c>
     </row>
     <row r="17">
@@ -1015,34 +1015,34 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.3324331214482134</v>
+        <v>0.3324532390318133</v>
       </c>
       <c r="C17" t="n">
-        <v>0.006849080984309197</v>
+        <v>0.007292183518287879</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0282335078677138</v>
+        <v>0.03169852339611974</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6688271529459379</v>
+        <v>0.666210806776644</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2346365805993203</v>
+        <v>0.2350671712303506</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3499851131981069</v>
+        <v>0.3488898913968693</v>
       </c>
       <c r="H17" t="n">
-        <v>0.005138798762503394</v>
+        <v>0.004473052747175785</v>
       </c>
       <c r="I17" t="n">
-        <v>0.03342351949484559</v>
+        <v>0.03369410449395942</v>
       </c>
       <c r="J17" t="n">
-        <v>0.614310131717667</v>
+        <v>0.6172441387564125</v>
       </c>
       <c r="K17" t="n">
-        <v>0.217624149991672</v>
+        <v>0.2184704319991826</v>
       </c>
     </row>
     <row r="18">
@@ -1050,34 +1050,34 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3310294730419462</v>
+        <v>0.3308079622008584</v>
       </c>
       <c r="C18" t="n">
-        <v>0.009002715646700771</v>
+        <v>0.009804255838092565</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03835139595654071</v>
+        <v>0.03917223253488587</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6755790040238502</v>
+        <v>0.6747192712207477</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2409777052090305</v>
+        <v>0.2412319198645754</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3438542674888264</v>
+        <v>0.3431026610461148</v>
       </c>
       <c r="H18" t="n">
-        <v>0.004974760079339682</v>
+        <v>0.009098134115780504</v>
       </c>
       <c r="I18" t="n">
-        <v>0.03808988783043018</v>
+        <v>0.04838028020907019</v>
       </c>
       <c r="J18" t="n">
-        <v>0.6182017225757316</v>
+        <v>0.6193596296774343</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2204221234951671</v>
+        <v>0.225612681334095</v>
       </c>
     </row>
     <row r="19">
@@ -1085,34 +1085,34 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3293599117208611</v>
+        <v>0.3292980001054027</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01016309555326504</v>
+        <v>0.01104139532431286</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04405934302146946</v>
+        <v>0.0465658159387272</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6804609008917478</v>
+        <v>0.6785856103211171</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2448944464888274</v>
+        <v>0.245397607194719</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3429701558568261</v>
+        <v>0.342330969192765</v>
       </c>
       <c r="H19" t="n">
-        <v>0.003530051556776978</v>
+        <v>0.007927579662186851</v>
       </c>
       <c r="I19" t="n">
-        <v>0.03134171289875173</v>
+        <v>0.04406791752272757</v>
       </c>
       <c r="J19" t="n">
-        <v>0.6154087142306724</v>
+        <v>0.6161150430701381</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2167601595620671</v>
+        <v>0.2227035134183508</v>
       </c>
     </row>
     <row r="20">
@@ -1120,34 +1120,34 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3293405253101479</v>
+        <v>0.3292613551020622</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01237953487996836</v>
+        <v>0.01209395392750705</v>
       </c>
       <c r="D20" t="n">
-        <v>0.05169703587122553</v>
+        <v>0.05377499816523126</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6814431444308046</v>
+        <v>0.6791995716227684</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2485065717273328</v>
+        <v>0.2483561745718356</v>
       </c>
       <c r="G20" t="n">
-        <v>0.348197876052423</v>
+        <v>0.3475162481719797</v>
       </c>
       <c r="H20" t="n">
-        <v>0.006383355962843229</v>
+        <v>0.01433267856414495</v>
       </c>
       <c r="I20" t="n">
-        <v>0.03776725980565938</v>
+        <v>0.07470237536339581</v>
       </c>
       <c r="J20" t="n">
-        <v>0.6181264864056708</v>
+        <v>0.6201491580452159</v>
       </c>
       <c r="K20" t="n">
-        <v>0.2207590340580578</v>
+        <v>0.2363947373242522</v>
       </c>
     </row>
     <row r="21">
@@ -1155,34 +1155,34 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3283932784741575</v>
+        <v>0.328438994220712</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01069270596933462</v>
+        <v>0.01440007389823331</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04774785561893151</v>
+        <v>0.05957199049034992</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6841659637775473</v>
+        <v>0.6817021384595644</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2475355084552712</v>
+        <v>0.2518914009493825</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3445241234519265</v>
+        <v>0.3436678173867139</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01102954972610283</v>
+        <v>0.009792544367607944</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0602949810185963</v>
+        <v>0.06410927799277315</v>
       </c>
       <c r="J21" t="n">
-        <v>0.6255639404194545</v>
+        <v>0.6267003919280573</v>
       </c>
       <c r="K21" t="n">
-        <v>0.2322961570547179</v>
+        <v>0.2335340714294795</v>
       </c>
     </row>
     <row r="22">
@@ -1190,34 +1190,34 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3273361206732013</v>
+        <v>0.3272597742351619</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01368609102107426</v>
+        <v>0.01537019077674319</v>
       </c>
       <c r="D22" t="n">
-        <v>0.05668828470719319</v>
+        <v>0.06055850524920035</v>
       </c>
       <c r="E22" t="n">
-        <v>0.6866637765334598</v>
+        <v>0.6850629907946486</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2523460507539091</v>
+        <v>0.253663895606864</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3418930281292308</v>
+        <v>0.3411330065943978</v>
       </c>
       <c r="H22" t="n">
-        <v>0.008034021114724565</v>
+        <v>0.01661877302945135</v>
       </c>
       <c r="I22" t="n">
-        <v>0.04242622259479994</v>
+        <v>0.08641342476293931</v>
       </c>
       <c r="J22" t="n">
-        <v>0.6239000176538274</v>
+        <v>0.6248219115966941</v>
       </c>
       <c r="K22" t="n">
-        <v>0.224786753787784</v>
+        <v>0.2426180364630283</v>
       </c>
     </row>
     <row r="23">
@@ -1225,34 +1225,34 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3270433125170795</v>
+        <v>0.3268841244280338</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01604426978454082</v>
+        <v>0.01753245523012784</v>
       </c>
       <c r="D23" t="n">
-        <v>0.06460214119720781</v>
+        <v>0.07003397670036757</v>
       </c>
       <c r="E23" t="n">
-        <v>0.6884982391622672</v>
+        <v>0.6871067209973574</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2563815500480053</v>
+        <v>0.2582243843092842</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3421447480266744</v>
+        <v>0.3412269706075842</v>
       </c>
       <c r="H23" t="n">
-        <v>0.01214670630487978</v>
+        <v>0.01399806862707353</v>
       </c>
       <c r="I23" t="n">
-        <v>0.06035645203288324</v>
+        <v>0.07498367596570328</v>
       </c>
       <c r="J23" t="n">
-        <v>0.6251081112935581</v>
+        <v>0.6271856684425894</v>
       </c>
       <c r="K23" t="n">
-        <v>0.2325370898771071</v>
+        <v>0.2387224710117888</v>
       </c>
     </row>
     <row r="24">
@@ -1260,34 +1260,34 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3262393474578857</v>
+        <v>0.3260273178192702</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01400695388257225</v>
+        <v>0.01575044027193298</v>
       </c>
       <c r="D24" t="n">
-        <v>0.06245621613475357</v>
+        <v>0.06638214152024936</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6929350488611721</v>
+        <v>0.6918068505889421</v>
       </c>
       <c r="F24" t="n">
-        <v>0.2564660729594993</v>
+        <v>0.2579798107937081</v>
       </c>
       <c r="G24" t="n">
-        <v>0.3427841175686229</v>
+        <v>0.3422047753225673</v>
       </c>
       <c r="H24" t="n">
-        <v>0.01296253531416927</v>
+        <v>0.01231234392802154</v>
       </c>
       <c r="I24" t="n">
-        <v>0.06930763900981346</v>
+        <v>0.07071197411003237</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6248302081027359</v>
+        <v>0.6261729343437172</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2357001274755729</v>
+        <v>0.236399084127257</v>
       </c>
     </row>
     <row r="25">
@@ -1295,34 +1295,34 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.3245767564936118</v>
+        <v>0.3245705887675285</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01979976957966771</v>
+        <v>0.01861990665722958</v>
       </c>
       <c r="D25" t="n">
-        <v>0.07722793963693864</v>
+        <v>0.07638160064346618</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6910228047353187</v>
+        <v>0.6897969694601183</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2626835046506417</v>
+        <v>0.2615994922536047</v>
       </c>
       <c r="G25" t="n">
-        <v>0.3387890999967402</v>
+        <v>0.3378760828213258</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01055589971819654</v>
+        <v>0.01297436753338264</v>
       </c>
       <c r="I25" t="n">
-        <v>0.05649670953547942</v>
+        <v>0.07274910857100346</v>
       </c>
       <c r="J25" t="n">
-        <v>0.627488051428874</v>
+        <v>0.6290244135962708</v>
       </c>
       <c r="K25" t="n">
-        <v>0.23151355356085</v>
+        <v>0.2382492965668856</v>
       </c>
     </row>
     <row r="26">
@@ -1330,34 +1330,34 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.3241882385178046</v>
+        <v>0.3242101821709763</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01761483858287996</v>
+        <v>0.02115169542054851</v>
       </c>
       <c r="D26" t="n">
-        <v>0.07197278665823303</v>
+        <v>0.08371332815570599</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6975016158186471</v>
+        <v>0.6950675878677043</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2623630803532533</v>
+        <v>0.2666442038146529</v>
       </c>
       <c r="G26" t="n">
-        <v>0.3413958698511124</v>
+        <v>0.3406614024530757</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01592108966546051</v>
+        <v>0.01332145195640946</v>
       </c>
       <c r="I26" t="n">
-        <v>0.07552089816603284</v>
+        <v>0.08807611676051566</v>
       </c>
       <c r="J26" t="n">
-        <v>0.6263685675745716</v>
+        <v>0.627943445615605</v>
       </c>
       <c r="K26" t="n">
-        <v>0.239270185135355</v>
+        <v>0.2431136714441767</v>
       </c>
     </row>
     <row r="27">
@@ -1365,34 +1365,34 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.3227765163914724</v>
+        <v>0.3227623003450307</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01549927519490528</v>
+        <v>0.01819715731267059</v>
       </c>
       <c r="D27" t="n">
-        <v>0.06789060933804154</v>
+        <v>0.07593073745159981</v>
       </c>
       <c r="E27" t="n">
-        <v>0.6994582100726241</v>
+        <v>0.6976612127345905</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2609493648685237</v>
+        <v>0.2639297024996203</v>
       </c>
       <c r="G27" t="n">
-        <v>0.3379985757849433</v>
+        <v>0.3370691321112893</v>
       </c>
       <c r="H27" t="n">
-        <v>0.01336705061324701</v>
+        <v>0.017641240444843</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0677250957327683</v>
+        <v>0.0888342540805989</v>
       </c>
       <c r="J27" t="n">
-        <v>0.6281530452372126</v>
+        <v>0.6311753949755704</v>
       </c>
       <c r="K27" t="n">
-        <v>0.236415063861076</v>
+        <v>0.2458836298336708</v>
       </c>
     </row>
     <row r="28">
@@ -1400,34 +1400,34 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.3211381374434991</v>
+        <v>0.3209509331394326</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0219305537474154</v>
+        <v>0.02368217061338893</v>
       </c>
       <c r="D28" t="n">
-        <v>0.09089903417940987</v>
+        <v>0.09357596313665403</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7015157593510093</v>
+        <v>0.7018858445757576</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2714484490926115</v>
+        <v>0.2730479927752669</v>
       </c>
       <c r="G28" t="n">
-        <v>0.3370354676788503</v>
+        <v>0.3365029963580045</v>
       </c>
       <c r="H28" t="n">
-        <v>0.01901253727814146</v>
+        <v>0.02129770230396459</v>
       </c>
       <c r="I28" t="n">
-        <v>0.08904559189539936</v>
+        <v>0.1050514056755388</v>
       </c>
       <c r="J28" t="n">
-        <v>0.6301065095959181</v>
+        <v>0.6310689190383533</v>
       </c>
       <c r="K28" t="n">
-        <v>0.2460548795898196</v>
+        <v>0.2524726756726189</v>
       </c>
     </row>
     <row r="29">
@@ -1435,34 +1435,34 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3218311626802791</v>
+        <v>0.3218475752933459</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02154365222552881</v>
+        <v>0.023252974548842</v>
       </c>
       <c r="D29" t="n">
-        <v>0.08691236555381679</v>
+        <v>0.09193758433925601</v>
       </c>
       <c r="E29" t="n">
-        <v>0.7003699074602419</v>
+        <v>0.6979285134267372</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2696086417465292</v>
+        <v>0.2710396907716118</v>
       </c>
       <c r="G29" t="n">
-        <v>0.3376923203468323</v>
+        <v>0.3369364142417908</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01517138810552829</v>
+        <v>0.01262897196522399</v>
       </c>
       <c r="I29" t="n">
-        <v>0.07186017665318924</v>
+        <v>0.0709771974853997</v>
       </c>
       <c r="J29" t="n">
-        <v>0.626485999388655</v>
+        <v>0.6292535272255105</v>
       </c>
       <c r="K29" t="n">
-        <v>0.2378391880491242</v>
+        <v>0.2376198988920447</v>
       </c>
     </row>
     <row r="30">
@@ -1470,34 +1470,34 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.3208880092610013</v>
+        <v>0.3208844688805667</v>
       </c>
       <c r="C30" t="n">
-        <v>0.02394145263417712</v>
+        <v>0.025888726610796</v>
       </c>
       <c r="D30" t="n">
-        <v>0.09385320783632307</v>
+        <v>0.1001003217070279</v>
       </c>
       <c r="E30" t="n">
-        <v>0.702775021580873</v>
+        <v>0.7022040671942502</v>
       </c>
       <c r="F30" t="n">
-        <v>0.2735232273504578</v>
+        <v>0.276064371837358</v>
       </c>
       <c r="G30" t="n">
-        <v>0.338222243569114</v>
+        <v>0.3374055041508241</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0160453830500526</v>
+        <v>0.01297188347471825</v>
       </c>
       <c r="I30" t="n">
-        <v>0.07848577199026076</v>
+        <v>0.07935813968984101</v>
       </c>
       <c r="J30" t="n">
-        <v>0.631083329094326</v>
+        <v>0.6330550828861631</v>
       </c>
       <c r="K30" t="n">
-        <v>0.2418714947115465</v>
+        <v>0.2417950353502408</v>
       </c>
     </row>
     <row r="31">
@@ -1505,34 +1505,34 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.3199734708124941</v>
+        <v>0.3198839514092965</v>
       </c>
       <c r="C31" t="n">
-        <v>0.02137512126910757</v>
+        <v>0.02302429643143859</v>
       </c>
       <c r="D31" t="n">
-        <v>0.08633924892963296</v>
+        <v>0.08977237928841941</v>
       </c>
       <c r="E31" t="n">
-        <v>0.7079649316220863</v>
+        <v>0.7062807523534133</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2718931006069423</v>
+        <v>0.2730258093577571</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3370052386413921</v>
+        <v>0.3364478728987954</v>
       </c>
       <c r="H31" t="n">
-        <v>0.01652272891849427</v>
+        <v>0.0166458952807203</v>
       </c>
       <c r="I31" t="n">
-        <v>0.08563558918713118</v>
+        <v>0.09169799590745228</v>
       </c>
       <c r="J31" t="n">
-        <v>0.6288295467471219</v>
+        <v>0.6293661891823457</v>
       </c>
       <c r="K31" t="n">
-        <v>0.2436626216175825</v>
+        <v>0.2459033601235061</v>
       </c>
     </row>
     <row r="32">
@@ -1540,34 +1540,34 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.3189429796554826</v>
+        <v>0.3189581947570497</v>
       </c>
       <c r="C32" t="n">
-        <v>0.02578627934624247</v>
+        <v>0.0274183642105713</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1045572568589149</v>
+        <v>0.1080869610392247</v>
       </c>
       <c r="E32" t="n">
-        <v>0.7083676973216051</v>
+        <v>0.7071678677657698</v>
       </c>
       <c r="F32" t="n">
-        <v>0.2795704111755875</v>
+        <v>0.2808910643385219</v>
       </c>
       <c r="G32" t="n">
-        <v>0.3353190638802268</v>
+        <v>0.3345482308756221</v>
       </c>
       <c r="H32" t="n">
-        <v>0.01672791664591243</v>
+        <v>0.01722129023779997</v>
       </c>
       <c r="I32" t="n">
-        <v>0.08551757365654929</v>
+        <v>0.09047526951832062</v>
       </c>
       <c r="J32" t="n">
-        <v>0.6300055702257568</v>
+        <v>0.6314567673892005</v>
       </c>
       <c r="K32" t="n">
-        <v>0.2440836868427395</v>
+        <v>0.2463844423817737</v>
       </c>
     </row>
     <row r="33">
@@ -1575,34 +1575,34 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.3195893923667344</v>
+        <v>0.3200319612568075</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0243608063722163</v>
+        <v>0.02445207054941474</v>
       </c>
       <c r="D33" t="n">
-        <v>0.09929495088816348</v>
+        <v>0.09934332058673732</v>
       </c>
       <c r="E33" t="n">
-        <v>0.7079649128291765</v>
+        <v>0.7046746263686983</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2772068900298521</v>
+        <v>0.2761566725016167</v>
       </c>
       <c r="G33" t="n">
-        <v>0.3362464796413075</v>
+        <v>0.3355643058365042</v>
       </c>
       <c r="H33" t="n">
-        <v>0.01817323046264537</v>
+        <v>0.02024889230074721</v>
       </c>
       <c r="I33" t="n">
-        <v>0.08200057391553876</v>
+        <v>0.0961398673871775</v>
       </c>
       <c r="J33" t="n">
-        <v>0.6335120494310704</v>
+        <v>0.6331052690087956</v>
       </c>
       <c r="K33" t="n">
-        <v>0.2445619512697515</v>
+        <v>0.2498313428989068</v>
       </c>
     </row>
     <row r="34">
@@ -1610,34 +1610,34 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.3192283077673478</v>
+        <v>0.3193213147195903</v>
       </c>
       <c r="C34" t="n">
-        <v>0.02675772374211946</v>
+        <v>0.02819674862782559</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1018492570705472</v>
+        <v>0.101440925187776</v>
       </c>
       <c r="E34" t="n">
-        <v>0.70892551258693</v>
+        <v>0.7072898128028473</v>
       </c>
       <c r="F34" t="n">
-        <v>0.2791774977998656</v>
+        <v>0.2789758288728163</v>
       </c>
       <c r="G34" t="n">
-        <v>0.3386058075861497</v>
+        <v>0.3378918306394057</v>
       </c>
       <c r="H34" t="n">
-        <v>0.01625873321424195</v>
+        <v>0.01615219077481175</v>
       </c>
       <c r="I34" t="n">
-        <v>0.09205958647279902</v>
+        <v>0.09688360781205688</v>
       </c>
       <c r="J34" t="n">
-        <v>0.62967996355316</v>
+        <v>0.631053553176389</v>
       </c>
       <c r="K34" t="n">
-        <v>0.2459994277467337</v>
+        <v>0.2480297839210859</v>
       </c>
     </row>
     <row r="35">
@@ -1645,34 +1645,34 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.3165868737480857</v>
+        <v>0.3166499628939412</v>
       </c>
       <c r="C35" t="n">
-        <v>0.03215815198310326</v>
+        <v>0.03303868732772722</v>
       </c>
       <c r="D35" t="n">
-        <v>0.10952933413359</v>
+        <v>0.1112045329632563</v>
       </c>
       <c r="E35" t="n">
-        <v>0.7144763053089204</v>
+        <v>0.7131195120205901</v>
       </c>
       <c r="F35" t="n">
-        <v>0.2853879304752046</v>
+        <v>0.2857875774371912</v>
       </c>
       <c r="G35" t="n">
-        <v>0.3415657918561589</v>
+        <v>0.3409245881167325</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0153070060703706</v>
+        <v>0.0162430559140835</v>
       </c>
       <c r="I35" t="n">
-        <v>0.08240798712362916</v>
+        <v>0.08857666926821564</v>
       </c>
       <c r="J35" t="n">
-        <v>0.6342518078979891</v>
+        <v>0.6363600816753578</v>
       </c>
       <c r="K35" t="n">
-        <v>0.2439889336973296</v>
+        <v>0.247059935619219</v>
       </c>
     </row>
     <row r="36">
@@ -1680,34 +1680,34 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.3160503235730258</v>
+        <v>0.3160647069188682</v>
       </c>
       <c r="C36" t="n">
-        <v>0.03193230933423022</v>
+        <v>0.03300174178863634</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1204423945049378</v>
+        <v>0.1194955921924849</v>
       </c>
       <c r="E36" t="n">
-        <v>0.7162269141551423</v>
+        <v>0.7156740746999735</v>
       </c>
       <c r="F36" t="n">
-        <v>0.2895338726647701</v>
+        <v>0.2893904695603649</v>
       </c>
       <c r="G36" t="n">
-        <v>0.3370787325230511</v>
+        <v>0.3363494900139896</v>
       </c>
       <c r="H36" t="n">
-        <v>0.02632048499977353</v>
+        <v>0.02344815472093818</v>
       </c>
       <c r="I36" t="n">
-        <v>0.09816035278531771</v>
+        <v>0.1091931935160585</v>
       </c>
       <c r="J36" t="n">
-        <v>0.6334244341051078</v>
+        <v>0.6360144246260084</v>
       </c>
       <c r="K36" t="n">
-        <v>0.2526350906300663</v>
+        <v>0.256218590954335</v>
       </c>
     </row>
     <row r="37">
@@ -1715,34 +1715,34 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.3159147609363903</v>
+        <v>0.3159568015147339</v>
       </c>
       <c r="C37" t="n">
-        <v>0.03594241317933215</v>
+        <v>0.03761940485322371</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1169158047556706</v>
+        <v>0.1186743698333279</v>
       </c>
       <c r="E37" t="n">
-        <v>0.71679120494076</v>
+        <v>0.7156504013154246</v>
       </c>
       <c r="F37" t="n">
-        <v>0.2898831409585876</v>
+        <v>0.2906480586673254</v>
       </c>
       <c r="G37" t="n">
-        <v>0.3354839885776693</v>
+        <v>0.3346066325902939</v>
       </c>
       <c r="H37" t="n">
-        <v>0.02609319055931157</v>
+        <v>0.02821813206521767</v>
       </c>
       <c r="I37" t="n">
-        <v>0.0795364999503988</v>
+        <v>0.09114384576648916</v>
       </c>
       <c r="J37" t="n">
-        <v>0.6385385513838975</v>
+        <v>0.6396915490194424</v>
       </c>
       <c r="K37" t="n">
-        <v>0.2480560806312026</v>
+        <v>0.2530178422837164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>